<commit_message>
Complete working page generation code and examples
</commit_message>
<xml_diff>
--- a/terms.xlsx
+++ b/terms.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/james_bartlett_glasgow_ac_uk/Documents/R Sandbox/Create RMd/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesbartlett/Documents/git_repos/sotl_glossary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F6AEBFE-EF0A-F74F-880D-C28ED50DC04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6A764C-4DBD-AC46-9670-A397B2A62FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="27040" windowHeight="16880" xr2:uid="{B196321C-ADC4-4A4A-87D3-273D6F0F0C26}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>term</t>
   </si>
@@ -53,25 +53,41 @@
     <t>A scholarly approach to teaching.</t>
   </si>
   <si>
-    <t>sotl</t>
-  </si>
-  <si>
-    <t>file_name</t>
-  </si>
-  <si>
     <t>SoTL, or the Scholarship of Teaching and Learning, is a scholarly approach to teaching that involves systematically examining one's own teaching practices and student learning to improve both, often with the goal of making findings public to contribute to the wider teaching community</t>
   </si>
   <si>
-    <t>impact</t>
-  </si>
-  <si>
-    <t>Impact</t>
-  </si>
-  <si>
-    <t>The demonstrable contribution that excellent research makes to society and the economy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The demonstable contribution of research. </t>
+    <t>Pedagogy</t>
+  </si>
+  <si>
+    <t>Active learning</t>
+  </si>
+  <si>
+    <t>Engagement</t>
+  </si>
+  <si>
+    <t>Autonomy</t>
+  </si>
+  <si>
+    <t>The method and practice of teaching, especially as an academic subject or theoretical concept.</t>
+  </si>
+  <si>
+    <t>The method and practice of teaching.</t>
+  </si>
+  <si>
+    <t>Active learning is a method of learning in which students are actively or experientially involved in the learning process.</t>
+  </si>
+  <si>
+    <t>Students actively involved in the learning process.</t>
+  </si>
+  <si>
+    <t>Psychological investiment in learning.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Autonomy means the ability to take control of one's own learning, independently or in collaboration with others.</t>
+  </si>
+  <si>
+    <t>Taking control of one's own learning.</t>
   </si>
 </sst>
 </file>
@@ -107,8 +123,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,54 +460,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D26857E-AF0E-5A4A-BDEA-8DC40A4832B4}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>